<commit_message>
exel file base instructions updated to first version of basis instructions
</commit_message>
<xml_diff>
--- a/docs/YYMMDD_A042_Base-Instructions_PF.xlsx
+++ b/docs/YYMMDD_A042_Base-Instructions_PF.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="87">
   <si>
     <t>Dummy</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Compas Frame 1, Compas Frame 2 ,External Axes, Speed, Zone</t>
-  </si>
-  <si>
-    <t>MoveJ / MoveL</t>
   </si>
   <si>
     <t>GetFrame</t>
@@ -440,12 +437,21 @@
   <si>
     <t>Robot Joints, External Axes</t>
   </si>
+  <si>
+    <t>Compas Frame [Point, Vector X, Vector Y]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MoveJ or L </t>
+  </si>
+  <si>
+    <t>MoveToFrameJ or L</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,19 +519,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,11 +537,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -553,9 +547,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -574,11 +567,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -860,12 +852,12 @@
   <dimension ref="A1:XEY30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="63.7109375" customWidth="1"/>
     <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
@@ -17261,16 +17253,16 @@
     </row>
     <row r="4" spans="1:16379" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>27</v>
@@ -17283,7 +17275,7 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C5" t="s">
@@ -17293,15 +17285,15 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>75</v>
+      <c r="B6" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -17313,17 +17305,17 @@
         <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
-        <v>50</v>
+      <c r="B7" s="9" t="s">
+        <v>49</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="8"/>
       <c r="D7" t="s">
         <v>15</v>
       </c>
@@ -17331,27 +17323,30 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>76</v>
+      <c r="B8" s="9" t="s">
+        <v>75</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="8"/>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
-        <v>79</v>
+      <c r="B9" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
@@ -17360,18 +17355,18 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
-      <c r="B10" t="s">
-        <v>80</v>
+      <c r="B10" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -17380,18 +17375,18 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
-      <c r="B11" t="s">
-        <v>81</v>
+      <c r="B11" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -17400,7 +17395,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:16379" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -17420,14 +17415,14 @@
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
@@ -17445,9 +17440,9 @@
     </row>
     <row r="14" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C14" t="s">
@@ -17465,9 +17460,9 @@
     </row>
     <row r="15" spans="1:16379" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C15" t="s">
@@ -17487,11 +17482,11 @@
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -17500,75 +17495,75 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B19" t="s">
-        <v>72</v>
-      </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="9" t="s">
         <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
         <v>19</v>
@@ -17577,18 +17572,18 @@
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
@@ -17597,18 +17592,18 @@
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="B22" t="s">
-        <v>51</v>
+      <c r="B22" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
@@ -17617,18 +17612,18 @@
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -17637,14 +17632,14 @@
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
@@ -17657,18 +17652,18 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="9" t="s">
         <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -17677,18 +17672,18 @@
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" t="s">
         <v>20</v>
@@ -17697,14 +17692,14 @@
         <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C27" t="s">
@@ -17717,14 +17712,14 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C28" t="s">
@@ -17737,14 +17732,14 @@
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C29" t="s">
@@ -17757,15 +17752,15 @@
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>